<commit_message>
Cleaning of the code
</commit_message>
<xml_diff>
--- a/conf.xlsx
+++ b/conf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\conf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\conferences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70C7EFA-0E02-4631-BB81-60C295C56A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BC187B-12CE-453F-869A-9E186A0DC35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="459">
   <si>
     <t>video_id</t>
   </si>
@@ -346,9 +346,6 @@
     <t>La génétique</t>
   </si>
   <si>
-    <t xml:space="preserve"> Darwin</t>
-  </si>
-  <si>
     <t>https://youtu.be/UrdPaxfrbqs?si=aXR1EIEC8sQ8ISqs</t>
   </si>
   <si>
@@ -826,9 +823,6 @@
     <t>Vivons-nous dans un multivers ?</t>
   </si>
   <si>
-    <t>Le Multivers</t>
-  </si>
-  <si>
     <t>https://youtu.be/PNMZHr3L_Ws?si=x408A9e95tlIGbQm</t>
   </si>
   <si>
@@ -862,9 +856,6 @@
     <t>Jean-Marc Jancovici</t>
   </si>
   <si>
-    <t>Transition energétique</t>
-  </si>
-  <si>
     <t xml:space="preserve">Economie </t>
   </si>
   <si>
@@ -1129,9 +1120,6 @@
     <t>Cedric Villani</t>
   </si>
   <si>
-    <t>Rigolo</t>
-  </si>
-  <si>
     <t>Strasbourg</t>
   </si>
   <si>
@@ -1391,6 +1379,24 @@
   </si>
   <si>
     <t>https://i.ytimg.com/vi/MSzQ8Fb6Y3s/hq720.jpg?v=662b76cc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OTXv9iZVRNg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conférence de Doctorat Honoris Causa </t>
+  </si>
+  <si>
+    <t>Université de Liège</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>La transition énergétique</t>
+  </si>
+  <si>
+    <t>Le multivers</t>
   </si>
 </sst>
 </file>
@@ -1449,12 +1455,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1757,28 +1764,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="188.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1787,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1814,22 +1822,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
@@ -1839,8 +1847,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>44144</v>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1855,22 +1863,22 @@
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
         <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
         <v>25</v>
+      </c>
+      <c r="P2" s="2">
+        <v>44144</v>
       </c>
       <c r="Q2" t="s">
         <v>26</v>
@@ -1880,8 +1888,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>42516</v>
+      <c r="B3" t="s">
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1899,22 +1907,22 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="s">
         <v>34</v>
+      </c>
+      <c r="P3" s="2">
+        <v>42516</v>
       </c>
       <c r="Q3" t="s">
         <v>35</v>
@@ -1924,8 +1932,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>42541</v>
+      <c r="B4" t="s">
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
@@ -1940,22 +1948,22 @@
         <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
         <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" t="s">
         <v>40</v>
+      </c>
+      <c r="P4" s="2">
+        <v>42541</v>
       </c>
       <c r="Q4" t="s">
         <v>41</v>
@@ -1965,8 +1973,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>42420</v>
+      <c r="B5" t="s">
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
@@ -1981,22 +1989,22 @@
         <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="N5" t="s">
         <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="s">
         <v>47</v>
+      </c>
+      <c r="P5" s="2">
+        <v>42420</v>
       </c>
       <c r="Q5" t="s">
         <v>48</v>
@@ -2006,8 +2014,8 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>44691</v>
+      <c r="B6" t="s">
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -2022,22 +2030,22 @@
         <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="N6" t="s">
         <v>24</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="s">
         <v>54</v>
+      </c>
+      <c r="P6" s="2">
+        <v>44691</v>
       </c>
       <c r="Q6" t="s">
         <v>55</v>
@@ -2047,8 +2055,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>41729</v>
+      <c r="B7" t="s">
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -2069,22 +2077,22 @@
         <v>59</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" t="s">
         <v>63</v>
+      </c>
+      <c r="P7" s="2">
+        <v>41729</v>
       </c>
       <c r="Q7" t="s">
         <v>64</v>
@@ -2094,8 +2102,8 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>45281</v>
+      <c r="B8" t="s">
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>65</v>
@@ -2113,22 +2121,22 @@
         <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="N8" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
-      </c>
-      <c r="P8" t="s">
         <v>71</v>
+      </c>
+      <c r="P8" s="2">
+        <v>45281</v>
       </c>
       <c r="Q8" t="s">
         <v>72</v>
@@ -2138,8 +2146,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>45041</v>
+      <c r="B9" t="s">
+        <v>76</v>
       </c>
       <c r="C9" t="s">
         <v>73</v>
@@ -2160,22 +2168,22 @@
         <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M9" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="N9" t="s">
         <v>24</v>
       </c>
       <c r="O9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" t="s">
         <v>79</v>
+      </c>
+      <c r="P9" s="2">
+        <v>45041</v>
       </c>
       <c r="Q9" t="s">
         <v>80</v>
@@ -2185,8 +2193,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>43369</v>
+      <c r="B10" t="s">
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>81</v>
@@ -2204,19 +2212,19 @@
         <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
-      </c>
-      <c r="L10" t="s">
         <v>85</v>
       </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
       <c r="N10" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="O10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P10" t="s">
         <v>86</v>
+      </c>
+      <c r="P10" s="2">
+        <v>43369</v>
       </c>
       <c r="Q10" t="s">
         <v>87</v>
@@ -2226,8 +2234,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>41939</v>
+      <c r="B11" t="s">
+        <v>92</v>
       </c>
       <c r="C11" t="s">
         <v>88</v>
@@ -2245,22 +2253,22 @@
         <v>91</v>
       </c>
       <c r="K11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M11" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="N11" t="s">
         <v>24</v>
       </c>
       <c r="O11" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" t="s">
         <v>95</v>
+      </c>
+      <c r="P11" s="2">
+        <v>41939</v>
       </c>
       <c r="Q11" t="s">
         <v>96</v>
@@ -2270,8 +2278,8 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>45349</v>
+      <c r="B12" t="s">
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>97</v>
@@ -2289,22 +2297,22 @@
         <v>99</v>
       </c>
       <c r="K12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M12" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="N12" t="s">
         <v>24</v>
       </c>
       <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" t="s">
         <v>103</v>
+      </c>
+      <c r="P12" s="2">
+        <v>45349</v>
       </c>
       <c r="Q12" t="s">
         <v>104</v>
@@ -2314,8 +2322,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <v>41813</v>
+      <c r="B13" t="s">
+        <v>108</v>
       </c>
       <c r="C13" t="s">
         <v>105</v>
@@ -2333,7 +2341,7 @@
         <v>107</v>
       </c>
       <c r="H13" t="s">
-        <v>108</v>
+        <v>456</v>
       </c>
       <c r="K13" t="s">
         <v>109</v>
@@ -2342,250 +2350,250 @@
         <v>110</v>
       </c>
       <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" t="s">
         <v>111</v>
       </c>
-      <c r="N13" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="P13" s="2">
+        <v>41813</v>
+      </c>
+      <c r="Q13" t="s">
         <v>112</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>39532</v>
+      <c r="B14" t="s">
+        <v>117</v>
       </c>
       <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
         <v>114</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
         <v>115</v>
       </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>116</v>
-      </c>
-      <c r="G14" t="s">
-        <v>117</v>
       </c>
       <c r="K14" t="s">
         <v>118</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
         <v>119</v>
-      </c>
-      <c r="N14" t="s">
-        <v>24</v>
       </c>
       <c r="O14" t="s">
         <v>120</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="2">
+        <v>39532</v>
+      </c>
+      <c r="Q14" t="s">
         <v>121</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <v>41966</v>
+      <c r="B15" t="s">
+        <v>124</v>
       </c>
       <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
         <v>123</v>
       </c>
-      <c r="D15" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>124</v>
-      </c>
       <c r="G15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K15" t="s">
         <v>125</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
+        <v>119</v>
+      </c>
+      <c r="N15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" t="s">
         <v>126</v>
       </c>
-      <c r="N15" t="s">
-        <v>120</v>
-      </c>
-      <c r="O15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="P15" s="2">
+        <v>41966</v>
+      </c>
+      <c r="Q15" t="s">
         <v>127</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <v>43404</v>
+      <c r="B16" t="s">
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K16" t="s">
         <v>130</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" t="s">
         <v>131</v>
       </c>
-      <c r="N16" t="s">
-        <v>24</v>
-      </c>
-      <c r="O16" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="P16" s="2">
+        <v>43404</v>
+      </c>
+      <c r="Q16" t="s">
         <v>132</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <v>45232</v>
+      <c r="B17" t="s">
+        <v>135</v>
       </c>
       <c r="C17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
         <v>134</v>
       </c>
-      <c r="D17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" t="s">
-        <v>135</v>
-      </c>
       <c r="G17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K17" t="s">
         <v>136</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" t="s">
         <v>137</v>
       </c>
-      <c r="N17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" t="s">
+      <c r="P17" s="2">
+        <v>45232</v>
+      </c>
+      <c r="Q17" t="s">
         <v>138</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" t="s">
+        <v>141</v>
+      </c>
+      <c r="K18" t="s">
+        <v>118</v>
+      </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" t="s">
+        <v>143</v>
+      </c>
+      <c r="P18" s="2">
         <v>45351</v>
       </c>
-      <c r="C18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" t="s">
-        <v>142</v>
-      </c>
-      <c r="K18" t="s">
-        <v>143</v>
-      </c>
-      <c r="L18" t="s">
-        <v>119</v>
-      </c>
-      <c r="N18" t="s">
-        <v>24</v>
-      </c>
-      <c r="O18" t="s">
-        <v>24</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>144</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <v>44540</v>
+      <c r="B19" t="s">
+        <v>149</v>
       </c>
       <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" t="s">
         <v>146</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
         <v>147</v>
       </c>
-      <c r="E19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>148</v>
-      </c>
-      <c r="G19" t="s">
-        <v>149</v>
       </c>
       <c r="K19" t="s">
         <v>150</v>
@@ -2594,80 +2602,83 @@
         <v>151</v>
       </c>
       <c r="M19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" t="s">
         <v>152</v>
       </c>
-      <c r="N19" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19" t="s">
-        <v>24</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="P19" s="2">
+        <v>44540</v>
+      </c>
+      <c r="Q19" t="s">
         <v>153</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>156</v>
+      </c>
+      <c r="K20" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P20" s="2">
         <v>42997</v>
       </c>
-      <c r="C20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" t="s">
-        <v>157</v>
-      </c>
-      <c r="K20" t="s">
-        <v>158</v>
-      </c>
-      <c r="L20" t="s">
-        <v>126</v>
-      </c>
-      <c r="M20" t="s">
-        <v>159</v>
-      </c>
-      <c r="N20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" t="s">
-        <v>24</v>
-      </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>160</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
-        <v>42852</v>
+      <c r="B21" t="s">
+        <v>162</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
         <v>156</v>
       </c>
-      <c r="E21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" t="s">
-        <v>157</v>
+      <c r="G21" t="s">
+        <v>246</v>
       </c>
       <c r="K21" t="s">
         <v>163</v>
@@ -2676,33 +2687,33 @@
         <v>164</v>
       </c>
       <c r="M21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" t="s">
         <v>165</v>
       </c>
-      <c r="N21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O21" t="s">
-        <v>24</v>
-      </c>
-      <c r="P21" t="s">
+      <c r="P21" s="2">
+        <v>42852</v>
+      </c>
+      <c r="Q21" t="s">
         <v>166</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
-        <v>43643</v>
+      <c r="B22" t="s">
+        <v>167</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -2711,42 +2722,42 @@
         <v>28</v>
       </c>
       <c r="K22" t="s">
+        <v>118</v>
+      </c>
+      <c r="M22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" t="s">
         <v>168</v>
-      </c>
-      <c r="L22" t="s">
-        <v>119</v>
-      </c>
-      <c r="N22" t="s">
-        <v>33</v>
       </c>
       <c r="O22" t="s">
         <v>169</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="2">
+        <v>43643</v>
+      </c>
+      <c r="Q22" t="s">
         <v>170</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <v>40813</v>
+      <c r="B23" t="s">
+        <v>173</v>
       </c>
       <c r="C23" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
         <v>172</v>
-      </c>
-      <c r="D23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" t="s">
-        <v>173</v>
       </c>
       <c r="K23" t="s">
         <v>174</v>
@@ -2755,121 +2766,121 @@
         <v>175</v>
       </c>
       <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" t="s">
         <v>176</v>
       </c>
-      <c r="N23" t="s">
-        <v>24</v>
-      </c>
-      <c r="O23" t="s">
-        <v>24</v>
-      </c>
-      <c r="P23" t="s">
+      <c r="P23" s="2">
+        <v>40813</v>
+      </c>
+      <c r="Q23" t="s">
         <v>177</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <v>43019</v>
+      <c r="B24" t="s">
+        <v>182</v>
       </c>
       <c r="C24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" t="s">
         <v>179</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
         <v>180</v>
       </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>181</v>
-      </c>
-      <c r="I24" t="s">
-        <v>182</v>
       </c>
       <c r="K24" t="s">
         <v>183</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O24" t="s">
         <v>184</v>
       </c>
-      <c r="N24" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" t="s">
-        <v>33</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="P24" s="2">
+        <v>43019</v>
+      </c>
+      <c r="Q24" t="s">
         <v>185</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
-        <v>42860</v>
+      <c r="B25" t="s">
+        <v>188</v>
       </c>
       <c r="C25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
         <v>187</v>
-      </c>
-      <c r="D25" t="s">
-        <v>180</v>
-      </c>
-      <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>188</v>
       </c>
       <c r="K25" t="s">
         <v>189</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" t="s">
         <v>190</v>
       </c>
-      <c r="N25" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" t="s">
-        <v>24</v>
-      </c>
-      <c r="P25" t="s">
+      <c r="P25" s="2">
+        <v>42860</v>
+      </c>
+      <c r="Q25" t="s">
         <v>191</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
-        <v>42791</v>
+      <c r="B26" t="s">
+        <v>195</v>
       </c>
       <c r="C26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D26" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
         <v>193</v>
       </c>
-      <c r="D26" t="s">
-        <v>180</v>
-      </c>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>194</v>
-      </c>
-      <c r="G26" t="s">
-        <v>195</v>
       </c>
       <c r="K26" t="s">
         <v>196</v>
@@ -2878,118 +2889,118 @@
         <v>197</v>
       </c>
       <c r="M26" t="s">
+        <v>24</v>
+      </c>
+      <c r="N26" t="s">
+        <v>33</v>
+      </c>
+      <c r="O26" t="s">
         <v>198</v>
       </c>
-      <c r="N26" t="s">
-        <v>24</v>
-      </c>
-      <c r="O26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="P26" s="2">
+        <v>42791</v>
+      </c>
+      <c r="Q26" t="s">
         <v>199</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
-        <v>42739</v>
+      <c r="B27" t="s">
+        <v>202</v>
       </c>
       <c r="C27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
         <v>201</v>
-      </c>
-      <c r="D27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" t="s">
-        <v>202</v>
       </c>
       <c r="K27" t="s">
         <v>203</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
+        <v>119</v>
+      </c>
+      <c r="N27" t="s">
+        <v>33</v>
+      </c>
+      <c r="O27" t="s">
         <v>204</v>
       </c>
-      <c r="N27" t="s">
-        <v>120</v>
-      </c>
-      <c r="O27" t="s">
-        <v>33</v>
-      </c>
-      <c r="P27" t="s">
+      <c r="P27" s="2">
+        <v>42739</v>
+      </c>
+      <c r="Q27" t="s">
         <v>205</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
-        <v>43021</v>
+      <c r="B28" t="s">
+        <v>208</v>
       </c>
       <c r="C28" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" t="s">
         <v>207</v>
-      </c>
-      <c r="D28" t="s">
-        <v>180</v>
-      </c>
-      <c r="E28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
-        <v>202</v>
-      </c>
-      <c r="I28" t="s">
-        <v>208</v>
       </c>
       <c r="K28" t="s">
         <v>209</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" t="s">
         <v>210</v>
       </c>
-      <c r="N28" t="s">
-        <v>24</v>
-      </c>
-      <c r="O28" t="s">
-        <v>33</v>
-      </c>
-      <c r="P28" t="s">
+      <c r="P28" s="2">
+        <v>43021</v>
+      </c>
+      <c r="Q28" t="s">
         <v>211</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
-        <v>43298</v>
+      <c r="B29" t="s">
+        <v>213</v>
       </c>
       <c r="C29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K29" t="s">
         <v>214</v>
@@ -2998,33 +3009,33 @@
         <v>215</v>
       </c>
       <c r="M29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" t="s">
         <v>216</v>
       </c>
-      <c r="N29" t="s">
-        <v>24</v>
-      </c>
-      <c r="O29" t="s">
-        <v>33</v>
-      </c>
-      <c r="P29" t="s">
+      <c r="P29" s="2">
+        <v>43298</v>
+      </c>
+      <c r="Q29" t="s">
         <v>217</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
-        <v>43426</v>
+      <c r="B30" t="s">
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
@@ -3033,10 +3044,10 @@
         <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K30" t="s">
         <v>221</v>
@@ -3045,74 +3056,74 @@
         <v>222</v>
       </c>
       <c r="M30" t="s">
+        <v>24</v>
+      </c>
+      <c r="N30" t="s">
+        <v>24</v>
+      </c>
+      <c r="O30" t="s">
         <v>223</v>
       </c>
-      <c r="N30" t="s">
-        <v>24</v>
-      </c>
-      <c r="O30" t="s">
-        <v>24</v>
-      </c>
-      <c r="P30" t="s">
+      <c r="P30" s="2">
+        <v>43426</v>
+      </c>
+      <c r="Q30" t="s">
         <v>224</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" t="s">
+        <v>228</v>
+      </c>
+      <c r="C31" t="s">
+        <v>225</v>
+      </c>
+      <c r="D31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" t="s">
+        <v>226</v>
+      </c>
+      <c r="I31" t="s">
+        <v>227</v>
+      </c>
+      <c r="K31" t="s">
+        <v>125</v>
+      </c>
+      <c r="M31" t="s">
+        <v>24</v>
+      </c>
+      <c r="N31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O31" t="s">
+        <v>229</v>
+      </c>
+      <c r="P31" s="2">
         <v>43448</v>
       </c>
-      <c r="C31" t="s">
-        <v>226</v>
-      </c>
-      <c r="D31" t="s">
-        <v>180</v>
-      </c>
-      <c r="E31" t="s">
-        <v>227</v>
-      </c>
-      <c r="F31" t="s">
-        <v>227</v>
-      </c>
-      <c r="I31" t="s">
-        <v>228</v>
-      </c>
-      <c r="K31" t="s">
-        <v>229</v>
-      </c>
-      <c r="L31" t="s">
-        <v>126</v>
-      </c>
-      <c r="N31" t="s">
-        <v>24</v>
-      </c>
-      <c r="O31" t="s">
-        <v>24</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>230</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
-        <v>43580</v>
+      <c r="B32" t="s">
+        <v>232</v>
       </c>
       <c r="C32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
@@ -3121,42 +3132,42 @@
         <v>29</v>
       </c>
       <c r="K32" t="s">
+        <v>118</v>
+      </c>
+      <c r="M32" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" t="s">
+        <v>33</v>
+      </c>
+      <c r="O32" t="s">
         <v>233</v>
       </c>
-      <c r="L32" t="s">
-        <v>119</v>
-      </c>
-      <c r="N32" t="s">
-        <v>24</v>
-      </c>
-      <c r="O32" t="s">
-        <v>33</v>
-      </c>
-      <c r="P32" t="s">
+      <c r="P32" s="2">
+        <v>43580</v>
+      </c>
+      <c r="Q32" t="s">
         <v>234</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
-        <v>43652</v>
+      <c r="B33" t="s">
+        <v>236</v>
       </c>
       <c r="C33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G33" t="s">
         <v>58</v>
@@ -3164,34 +3175,34 @@
       <c r="K33" t="s">
         <v>237</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" t="s">
+        <v>33</v>
+      </c>
+      <c r="O33" t="s">
         <v>238</v>
       </c>
-      <c r="N33" t="s">
-        <v>24</v>
-      </c>
-      <c r="O33" t="s">
-        <v>33</v>
-      </c>
-      <c r="P33" t="s">
+      <c r="P33" s="2">
+        <v>43652</v>
+      </c>
+      <c r="Q33" t="s">
         <v>239</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
-        <v>43838</v>
+      <c r="B34" t="s">
+        <v>241</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -3202,34 +3213,34 @@
       <c r="K34" t="s">
         <v>242</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N34" t="s">
+        <v>33</v>
+      </c>
+      <c r="O34" t="s">
         <v>243</v>
       </c>
-      <c r="N34" t="s">
-        <v>24</v>
-      </c>
-      <c r="O34" t="s">
-        <v>33</v>
-      </c>
-      <c r="P34" t="s">
+      <c r="P34" s="2">
+        <v>43838</v>
+      </c>
+      <c r="Q34" t="s">
         <v>244</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
-        <v>43869</v>
+      <c r="B35" t="s">
+        <v>248</v>
       </c>
       <c r="C35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -3238,42 +3249,42 @@
         <v>99</v>
       </c>
       <c r="G35" t="s">
+        <v>246</v>
+      </c>
+      <c r="I35" t="s">
         <v>247</v>
-      </c>
-      <c r="I35" t="s">
-        <v>248</v>
       </c>
       <c r="K35" t="s">
         <v>249</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" t="s">
+        <v>33</v>
+      </c>
+      <c r="O35" t="s">
         <v>250</v>
       </c>
-      <c r="N35" t="s">
-        <v>24</v>
-      </c>
-      <c r="O35" t="s">
-        <v>33</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="P35" s="2">
+        <v>43869</v>
+      </c>
+      <c r="Q35" t="s">
         <v>251</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
-        <v>44893</v>
+      <c r="B36" t="s">
+        <v>255</v>
       </c>
       <c r="C36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
@@ -3282,10 +3293,10 @@
         <v>99</v>
       </c>
       <c r="G36" t="s">
+        <v>253</v>
+      </c>
+      <c r="I36" t="s">
         <v>254</v>
-      </c>
-      <c r="I36" t="s">
-        <v>255</v>
       </c>
       <c r="K36" t="s">
         <v>256</v>
@@ -3294,33 +3305,33 @@
         <v>257</v>
       </c>
       <c r="M36" t="s">
+        <v>24</v>
+      </c>
+      <c r="N36" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" t="s">
         <v>258</v>
       </c>
-      <c r="N36" t="s">
-        <v>24</v>
-      </c>
-      <c r="O36" t="s">
-        <v>24</v>
-      </c>
-      <c r="P36" t="s">
+      <c r="P36" s="2">
+        <v>44893</v>
+      </c>
+      <c r="Q36" t="s">
         <v>259</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
-        <v>44972</v>
+      <c r="B37" t="s">
+        <v>262</v>
       </c>
       <c r="C37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -3329,80 +3340,80 @@
         <v>99</v>
       </c>
       <c r="I37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K37" t="s">
         <v>263</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N37" t="s">
+        <v>33</v>
+      </c>
+      <c r="O37" t="s">
         <v>264</v>
       </c>
-      <c r="N37" t="s">
-        <v>24</v>
-      </c>
-      <c r="O37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P37" t="s">
+      <c r="P37" s="2">
+        <v>44972</v>
+      </c>
+      <c r="Q37" t="s">
         <v>265</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
-        <v>42736</v>
+      <c r="B38" t="s">
+        <v>267</v>
       </c>
       <c r="C38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>268</v>
+        <v>458</v>
       </c>
       <c r="G38" t="s">
         <v>58</v>
       </c>
       <c r="K38" t="s">
+        <v>268</v>
+      </c>
+      <c r="M38" t="s">
+        <v>24</v>
+      </c>
+      <c r="N38" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" t="s">
         <v>269</v>
       </c>
-      <c r="L38" t="s">
+      <c r="P38" s="2">
+        <v>42736</v>
+      </c>
+      <c r="Q38" t="s">
         <v>270</v>
-      </c>
-      <c r="N38" t="s">
-        <v>24</v>
-      </c>
-      <c r="O38" t="s">
-        <v>33</v>
-      </c>
-      <c r="P38" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
-        <v>45315</v>
+      <c r="B39" t="s">
+        <v>272</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
@@ -3414,212 +3425,212 @@
         <v>74</v>
       </c>
       <c r="K39" t="s">
+        <v>273</v>
+      </c>
+      <c r="M39" t="s">
+        <v>24</v>
+      </c>
+      <c r="N39" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" t="s">
         <v>274</v>
       </c>
-      <c r="L39" t="s">
+      <c r="P39" s="2">
+        <v>45315</v>
+      </c>
+      <c r="Q39" t="s">
         <v>275</v>
-      </c>
-      <c r="N39" t="s">
-        <v>24</v>
-      </c>
-      <c r="O39" t="s">
-        <v>24</v>
-      </c>
-      <c r="P39" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" t="s">
+        <v>280</v>
+      </c>
+      <c r="C40" t="s">
+        <v>276</v>
+      </c>
+      <c r="D40" t="s">
+        <v>277</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>457</v>
+      </c>
+      <c r="G40" t="s">
+        <v>278</v>
+      </c>
+      <c r="H40" t="s">
+        <v>141</v>
+      </c>
+      <c r="I40" t="s">
+        <v>279</v>
+      </c>
+      <c r="K40" t="s">
+        <v>281</v>
+      </c>
+      <c r="L40" t="s">
+        <v>282</v>
+      </c>
+      <c r="M40" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" t="s">
+        <v>33</v>
+      </c>
+      <c r="O40" t="s">
+        <v>283</v>
+      </c>
+      <c r="P40" s="2">
         <v>43706</v>
       </c>
-      <c r="C40" t="s">
-        <v>278</v>
-      </c>
-      <c r="D40" t="s">
-        <v>279</v>
-      </c>
-      <c r="E40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>280</v>
-      </c>
-      <c r="G40" t="s">
-        <v>281</v>
-      </c>
-      <c r="H40" t="s">
-        <v>142</v>
-      </c>
-      <c r="I40" t="s">
-        <v>282</v>
-      </c>
-      <c r="K40" t="s">
-        <v>283</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="Q40" t="s">
         <v>284</v>
-      </c>
-      <c r="M40" t="s">
-        <v>285</v>
-      </c>
-      <c r="N40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O40" t="s">
-        <v>33</v>
-      </c>
-      <c r="P40" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C41" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41" t="s">
+        <v>277</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>457</v>
+      </c>
+      <c r="G41" t="s">
+        <v>278</v>
+      </c>
+      <c r="H41" t="s">
+        <v>141</v>
+      </c>
+      <c r="I41" t="s">
+        <v>286</v>
+      </c>
+      <c r="K41" t="s">
+        <v>288</v>
+      </c>
+      <c r="L41" t="s">
+        <v>289</v>
+      </c>
+      <c r="M41" t="s">
+        <v>24</v>
+      </c>
+      <c r="N41" t="s">
+        <v>33</v>
+      </c>
+      <c r="O41" t="s">
+        <v>290</v>
+      </c>
+      <c r="P41" s="2">
         <v>44445</v>
       </c>
-      <c r="C41" t="s">
-        <v>288</v>
-      </c>
-      <c r="D41" t="s">
-        <v>279</v>
-      </c>
-      <c r="E41" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
-        <v>280</v>
-      </c>
-      <c r="G41" t="s">
-        <v>281</v>
-      </c>
-      <c r="H41" t="s">
-        <v>142</v>
-      </c>
-      <c r="I41" t="s">
-        <v>289</v>
-      </c>
-      <c r="K41" t="s">
-        <v>290</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="Q41" t="s">
         <v>291</v>
-      </c>
-      <c r="M41" t="s">
-        <v>292</v>
-      </c>
-      <c r="N41" t="s">
-        <v>24</v>
-      </c>
-      <c r="O41" t="s">
-        <v>33</v>
-      </c>
-      <c r="P41" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" t="s">
+        <v>293</v>
+      </c>
+      <c r="C42" t="s">
+        <v>292</v>
+      </c>
+      <c r="D42" t="s">
+        <v>277</v>
+      </c>
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>457</v>
+      </c>
+      <c r="G42" t="s">
+        <v>278</v>
+      </c>
+      <c r="H42" t="s">
+        <v>141</v>
+      </c>
+      <c r="K42" t="s">
+        <v>294</v>
+      </c>
+      <c r="O42" t="s">
+        <v>295</v>
+      </c>
+      <c r="P42" s="2">
         <v>45246</v>
       </c>
-      <c r="C42" t="s">
-        <v>295</v>
-      </c>
-      <c r="D42" t="s">
-        <v>279</v>
-      </c>
-      <c r="E42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
-        <v>280</v>
-      </c>
-      <c r="G42" t="s">
-        <v>281</v>
-      </c>
-      <c r="H42" t="s">
-        <v>142</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="Q42" t="s">
         <v>296</v>
-      </c>
-      <c r="L42" t="s">
-        <v>297</v>
-      </c>
-      <c r="P42" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" t="s">
+        <v>300</v>
+      </c>
+      <c r="C43" t="s">
+        <v>297</v>
+      </c>
+      <c r="D43" t="s">
+        <v>298</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>299</v>
+      </c>
+      <c r="K43" t="s">
+        <v>203</v>
+      </c>
+      <c r="M43" t="s">
+        <v>24</v>
+      </c>
+      <c r="N43" t="s">
+        <v>24</v>
+      </c>
+      <c r="O43" t="s">
+        <v>301</v>
+      </c>
+      <c r="P43" s="2">
         <v>42736</v>
       </c>
-      <c r="C43" t="s">
-        <v>300</v>
-      </c>
-      <c r="D43" t="s">
-        <v>301</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="Q43" t="s">
         <v>302</v>
-      </c>
-      <c r="K43" t="s">
-        <v>303</v>
-      </c>
-      <c r="L43" t="s">
-        <v>204</v>
-      </c>
-      <c r="N43" t="s">
-        <v>24</v>
-      </c>
-      <c r="O43" t="s">
-        <v>24</v>
-      </c>
-      <c r="P43" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
-        <v>44204</v>
+      <c r="B44" t="s">
+        <v>306</v>
       </c>
       <c r="C44" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D44" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
@@ -3628,45 +3639,45 @@
         <v>99</v>
       </c>
       <c r="G44" t="s">
+        <v>304</v>
+      </c>
+      <c r="I44" t="s">
+        <v>305</v>
+      </c>
+      <c r="K44" t="s">
         <v>307</v>
       </c>
-      <c r="I44" t="s">
+      <c r="L44" t="s">
         <v>308</v>
       </c>
-      <c r="K44" t="s">
-        <v>309</v>
-      </c>
-      <c r="L44" t="s">
-        <v>310</v>
-      </c>
       <c r="M44" t="s">
-        <v>311</v>
+        <v>33</v>
       </c>
       <c r="N44" t="s">
         <v>33</v>
       </c>
       <c r="O44" t="s">
-        <v>33</v>
-      </c>
-      <c r="P44" t="s">
-        <v>312</v>
+        <v>309</v>
+      </c>
+      <c r="P44" s="2">
+        <v>44204</v>
       </c>
       <c r="Q44" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
-        <v>44882</v>
+      <c r="B45" t="s">
+        <v>313</v>
       </c>
       <c r="C45" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D45" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
@@ -3675,177 +3686,177 @@
         <v>99</v>
       </c>
       <c r="G45" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I45" t="s">
+        <v>312</v>
+      </c>
+      <c r="K45" t="s">
+        <v>314</v>
+      </c>
+      <c r="L45" t="s">
         <v>315</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" t="s">
+        <v>24</v>
+      </c>
+      <c r="O45" t="s">
         <v>316</v>
       </c>
-      <c r="L45" t="s">
+      <c r="P45" s="2">
+        <v>44882</v>
+      </c>
+      <c r="Q45" t="s">
         <v>317</v>
-      </c>
-      <c r="M45" t="s">
-        <v>318</v>
-      </c>
-      <c r="N45" t="s">
-        <v>33</v>
-      </c>
-      <c r="O45" t="s">
-        <v>24</v>
-      </c>
-      <c r="P45" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
-        <v>44866</v>
+      <c r="B46" t="s">
+        <v>319</v>
       </c>
       <c r="C46" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D46" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
         <v>99</v>
       </c>
       <c r="G46" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K46" t="s">
+        <v>320</v>
+      </c>
+      <c r="M46" t="s">
+        <v>24</v>
+      </c>
+      <c r="N46" t="s">
+        <v>24</v>
+      </c>
+      <c r="O46" t="s">
+        <v>321</v>
+      </c>
+      <c r="P46" s="2">
+        <v>44866</v>
+      </c>
+      <c r="Q46" t="s">
         <v>322</v>
-      </c>
-      <c r="L46" t="s">
-        <v>323</v>
-      </c>
-      <c r="N46" t="s">
-        <v>24</v>
-      </c>
-      <c r="O46" t="s">
-        <v>24</v>
-      </c>
-      <c r="P46" t="s">
-        <v>324</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" t="s">
+        <v>327</v>
+      </c>
+      <c r="C47" t="s">
+        <v>323</v>
+      </c>
+      <c r="D47" t="s">
+        <v>298</v>
+      </c>
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
+        <v>324</v>
+      </c>
+      <c r="G47" t="s">
+        <v>325</v>
+      </c>
+      <c r="J47" t="s">
+        <v>326</v>
+      </c>
+      <c r="K47" t="s">
+        <v>328</v>
+      </c>
+      <c r="L47" t="s">
+        <v>329</v>
+      </c>
+      <c r="M47" t="s">
+        <v>24</v>
+      </c>
+      <c r="N47" t="s">
+        <v>24</v>
+      </c>
+      <c r="O47" t="s">
+        <v>330</v>
+      </c>
+      <c r="P47" s="2">
         <v>44383</v>
       </c>
-      <c r="C47" t="s">
-        <v>326</v>
-      </c>
-      <c r="D47" t="s">
-        <v>301</v>
-      </c>
-      <c r="E47" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" t="s">
-        <v>327</v>
-      </c>
-      <c r="G47" t="s">
-        <v>328</v>
-      </c>
-      <c r="J47" t="s">
-        <v>329</v>
-      </c>
-      <c r="K47" t="s">
-        <v>330</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="Q47" t="s">
         <v>331</v>
-      </c>
-      <c r="M47" t="s">
-        <v>332</v>
-      </c>
-      <c r="N47" t="s">
-        <v>24</v>
-      </c>
-      <c r="O47" t="s">
-        <v>24</v>
-      </c>
-      <c r="P47" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
-        <v>43544</v>
+      <c r="B48" t="s">
+        <v>333</v>
       </c>
       <c r="C48" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D48" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F48" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G48" t="s">
         <v>99</v>
       </c>
       <c r="I48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K48" t="s">
-        <v>336</v>
-      </c>
-      <c r="L48" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="M48" t="s">
+        <v>24</v>
       </c>
       <c r="N48" t="s">
         <v>24</v>
       </c>
       <c r="O48" t="s">
-        <v>24</v>
-      </c>
-      <c r="P48" t="s">
-        <v>337</v>
+        <v>334</v>
+      </c>
+      <c r="P48" s="2">
+        <v>43544</v>
       </c>
       <c r="Q48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
-        <v>41948</v>
+      <c r="B49" t="s">
+        <v>338</v>
       </c>
       <c r="C49" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D49" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
@@ -3857,45 +3868,45 @@
         <v>59</v>
       </c>
       <c r="K49" t="s">
+        <v>339</v>
+      </c>
+      <c r="L49" t="s">
+        <v>340</v>
+      </c>
+      <c r="M49" t="s">
+        <v>24</v>
+      </c>
+      <c r="N49" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" t="s">
+        <v>258</v>
+      </c>
+      <c r="P49" s="2">
+        <v>41948</v>
+      </c>
+      <c r="Q49" t="s">
         <v>341</v>
-      </c>
-      <c r="L49" t="s">
-        <v>342</v>
-      </c>
-      <c r="M49" t="s">
-        <v>343</v>
-      </c>
-      <c r="N49" t="s">
-        <v>24</v>
-      </c>
-      <c r="O49" t="s">
-        <v>24</v>
-      </c>
-      <c r="P49" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="2">
-        <v>43013</v>
+      <c r="B50" t="s">
+        <v>344</v>
       </c>
       <c r="C50" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D50" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E50" t="s">
         <v>19</v>
       </c>
       <c r="F50" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G50" t="s">
         <v>58</v>
@@ -3904,39 +3915,39 @@
         <v>59</v>
       </c>
       <c r="K50" t="s">
+        <v>345</v>
+      </c>
+      <c r="L50" t="s">
+        <v>346</v>
+      </c>
+      <c r="M50" t="s">
+        <v>24</v>
+      </c>
+      <c r="N50" t="s">
+        <v>24</v>
+      </c>
+      <c r="O50" t="s">
+        <v>110</v>
+      </c>
+      <c r="P50" s="2">
+        <v>43013</v>
+      </c>
+      <c r="Q50" t="s">
         <v>347</v>
-      </c>
-      <c r="L50" t="s">
-        <v>348</v>
-      </c>
-      <c r="M50" t="s">
-        <v>349</v>
-      </c>
-      <c r="N50" t="s">
-        <v>24</v>
-      </c>
-      <c r="O50" t="s">
-        <v>24</v>
-      </c>
-      <c r="P50" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
-        <v>42816</v>
+      <c r="B51" t="s">
+        <v>351</v>
       </c>
       <c r="C51" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D51" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E51" t="s">
         <v>19</v>
@@ -3945,227 +3956,227 @@
         <v>106</v>
       </c>
       <c r="G51" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I51" t="s">
         <v>59</v>
       </c>
       <c r="K51" t="s">
+        <v>352</v>
+      </c>
+      <c r="L51" t="s">
+        <v>353</v>
+      </c>
+      <c r="M51" t="s">
+        <v>24</v>
+      </c>
+      <c r="N51" t="s">
+        <v>24</v>
+      </c>
+      <c r="O51" t="s">
         <v>354</v>
       </c>
-      <c r="L51" t="s">
+      <c r="P51" s="2">
+        <v>42816</v>
+      </c>
+      <c r="Q51" t="s">
         <v>355</v>
-      </c>
-      <c r="M51" t="s">
-        <v>356</v>
-      </c>
-      <c r="N51" t="s">
-        <v>24</v>
-      </c>
-      <c r="O51" t="s">
-        <v>24</v>
-      </c>
-      <c r="P51" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="2">
-        <v>41942</v>
+      <c r="B52" t="s">
+        <v>359</v>
       </c>
       <c r="C52" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D52" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I52" t="s">
         <v>59</v>
       </c>
       <c r="K52" t="s">
+        <v>360</v>
+      </c>
+      <c r="L52" t="s">
+        <v>361</v>
+      </c>
+      <c r="M52" t="s">
+        <v>24</v>
+      </c>
+      <c r="N52" t="s">
+        <v>24</v>
+      </c>
+      <c r="O52" t="s">
         <v>362</v>
       </c>
-      <c r="L52" t="s">
+      <c r="P52" s="2">
+        <v>41942</v>
+      </c>
+      <c r="Q52" t="s">
         <v>363</v>
-      </c>
-      <c r="M52" t="s">
-        <v>364</v>
-      </c>
-      <c r="N52" t="s">
-        <v>24</v>
-      </c>
-      <c r="O52" t="s">
-        <v>24</v>
-      </c>
-      <c r="P52" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" t="s">
+        <v>367</v>
+      </c>
+      <c r="C53" t="s">
+        <v>364</v>
+      </c>
+      <c r="D53" t="s">
+        <v>365</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" t="s">
+        <v>366</v>
+      </c>
+      <c r="K53" t="s">
+        <v>288</v>
+      </c>
+      <c r="L53" t="s">
+        <v>368</v>
+      </c>
+      <c r="M53" t="s">
+        <v>24</v>
+      </c>
+      <c r="N53" t="s">
+        <v>33</v>
+      </c>
+      <c r="O53" t="s">
+        <v>369</v>
+      </c>
+      <c r="P53" s="2">
         <v>41772</v>
       </c>
-      <c r="C53" t="s">
-        <v>367</v>
-      </c>
-      <c r="D53" t="s">
-        <v>368</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>369</v>
-      </c>
-      <c r="I53" t="s">
+      <c r="Q53" t="s">
         <v>370</v>
-      </c>
-      <c r="K53" t="s">
-        <v>371</v>
-      </c>
-      <c r="L53" t="s">
-        <v>291</v>
-      </c>
-      <c r="M53" t="s">
-        <v>372</v>
-      </c>
-      <c r="N53" t="s">
-        <v>24</v>
-      </c>
-      <c r="O53" t="s">
-        <v>33</v>
-      </c>
-      <c r="P53" t="s">
-        <v>373</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" t="s">
+        <v>372</v>
+      </c>
+      <c r="C54" t="s">
+        <v>371</v>
+      </c>
+      <c r="D54" t="s">
+        <v>365</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
+        <v>358</v>
+      </c>
+      <c r="G54" t="s">
+        <v>194</v>
+      </c>
+      <c r="I54" t="s">
+        <v>305</v>
+      </c>
+      <c r="K54" t="s">
+        <v>373</v>
+      </c>
+      <c r="L54" t="s">
+        <v>374</v>
+      </c>
+      <c r="M54" t="s">
+        <v>24</v>
+      </c>
+      <c r="N54" t="s">
+        <v>24</v>
+      </c>
+      <c r="O54" t="s">
+        <v>375</v>
+      </c>
+      <c r="P54" s="2">
         <v>42046</v>
       </c>
-      <c r="C54" t="s">
-        <v>375</v>
-      </c>
-      <c r="D54" t="s">
-        <v>368</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
-        <v>361</v>
-      </c>
-      <c r="G54" t="s">
-        <v>195</v>
-      </c>
-      <c r="I54" t="s">
-        <v>308</v>
-      </c>
-      <c r="K54" t="s">
+      <c r="Q54" t="s">
         <v>376</v>
-      </c>
-      <c r="L54" t="s">
-        <v>377</v>
-      </c>
-      <c r="M54" t="s">
-        <v>378</v>
-      </c>
-      <c r="N54" t="s">
-        <v>24</v>
-      </c>
-      <c r="O54" t="s">
-        <v>24</v>
-      </c>
-      <c r="P54" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="2">
-        <v>41939</v>
+      <c r="B55" t="s">
+        <v>379</v>
       </c>
       <c r="C55" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D55" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G55" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I55" t="s">
         <v>59</v>
       </c>
       <c r="K55" t="s">
+        <v>380</v>
+      </c>
+      <c r="L55" t="s">
+        <v>381</v>
+      </c>
+      <c r="M55" t="s">
+        <v>24</v>
+      </c>
+      <c r="N55" t="s">
+        <v>24</v>
+      </c>
+      <c r="O55" t="s">
+        <v>382</v>
+      </c>
+      <c r="P55" s="2">
+        <v>41939</v>
+      </c>
+      <c r="Q55" t="s">
         <v>383</v>
-      </c>
-      <c r="L55" t="s">
-        <v>384</v>
-      </c>
-      <c r="M55" t="s">
-        <v>385</v>
-      </c>
-      <c r="N55" t="s">
-        <v>24</v>
-      </c>
-      <c r="O55" t="s">
-        <v>24</v>
-      </c>
-      <c r="P55" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="2">
-        <v>40295</v>
+      <c r="B56" t="s">
+        <v>386</v>
       </c>
       <c r="C56" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D56" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E56" t="s">
         <v>19</v>
@@ -4177,332 +4188,338 @@
         <v>59</v>
       </c>
       <c r="K56" t="s">
+        <v>387</v>
+      </c>
+      <c r="L56" t="s">
+        <v>388</v>
+      </c>
+      <c r="M56" t="s">
+        <v>33</v>
+      </c>
+      <c r="N56" t="s">
+        <v>24</v>
+      </c>
+      <c r="O56" t="s">
+        <v>389</v>
+      </c>
+      <c r="P56" s="2">
+        <v>40295</v>
+      </c>
+      <c r="Q56" t="s">
         <v>390</v>
-      </c>
-      <c r="L56" t="s">
-        <v>391</v>
-      </c>
-      <c r="M56" t="s">
-        <v>392</v>
-      </c>
-      <c r="N56" t="s">
-        <v>33</v>
-      </c>
-      <c r="O56" t="s">
-        <v>24</v>
-      </c>
-      <c r="P56" t="s">
-        <v>393</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="2">
-        <v>44141</v>
+      <c r="B57" t="s">
+        <v>392</v>
       </c>
       <c r="C57" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D57" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F57" t="s">
         <v>58</v>
       </c>
       <c r="K57" t="s">
-        <v>396</v>
-      </c>
-      <c r="L57" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="M57" t="s">
+        <v>24</v>
       </c>
       <c r="N57" t="s">
         <v>24</v>
       </c>
       <c r="O57" t="s">
-        <v>24</v>
-      </c>
-      <c r="P57" t="s">
-        <v>397</v>
+        <v>393</v>
+      </c>
+      <c r="P57" s="2">
+        <v>44141</v>
       </c>
       <c r="Q57" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="2">
-        <v>42025</v>
+      <c r="B58" t="s">
+        <v>398</v>
       </c>
       <c r="C58" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D58" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I58" t="s">
         <v>59</v>
       </c>
       <c r="K58" t="s">
+        <v>399</v>
+      </c>
+      <c r="L58" t="s">
+        <v>400</v>
+      </c>
+      <c r="M58" t="s">
+        <v>24</v>
+      </c>
+      <c r="N58" t="s">
+        <v>24</v>
+      </c>
+      <c r="O58" t="s">
+        <v>401</v>
+      </c>
+      <c r="P58" s="2">
+        <v>42025</v>
+      </c>
+      <c r="Q58" t="s">
         <v>402</v>
-      </c>
-      <c r="L58" t="s">
-        <v>403</v>
-      </c>
-      <c r="M58" t="s">
-        <v>404</v>
-      </c>
-      <c r="N58" t="s">
-        <v>24</v>
-      </c>
-      <c r="O58" t="s">
-        <v>24</v>
-      </c>
-      <c r="P58" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
-        <v>41932</v>
+      <c r="B59" t="s">
+        <v>404</v>
       </c>
       <c r="C59" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D59" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G59" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I59" t="s">
         <v>59</v>
       </c>
       <c r="K59" t="s">
+        <v>405</v>
+      </c>
+      <c r="L59" t="s">
+        <v>406</v>
+      </c>
+      <c r="M59" t="s">
+        <v>24</v>
+      </c>
+      <c r="N59" t="s">
+        <v>24</v>
+      </c>
+      <c r="O59" t="s">
+        <v>407</v>
+      </c>
+      <c r="P59" s="2">
+        <v>41932</v>
+      </c>
+      <c r="Q59" t="s">
         <v>408</v>
-      </c>
-      <c r="L59" t="s">
-        <v>409</v>
-      </c>
-      <c r="M59" t="s">
-        <v>410</v>
-      </c>
-      <c r="N59" t="s">
-        <v>24</v>
-      </c>
-      <c r="O59" t="s">
-        <v>24</v>
-      </c>
-      <c r="P59" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="2">
-        <v>43061</v>
+      <c r="B60" t="s">
+        <v>411</v>
       </c>
       <c r="C60" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D60" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I60" t="s">
         <v>59</v>
       </c>
       <c r="K60" t="s">
+        <v>412</v>
+      </c>
+      <c r="L60" t="s">
+        <v>413</v>
+      </c>
+      <c r="M60" t="s">
+        <v>24</v>
+      </c>
+      <c r="N60" t="s">
+        <v>24</v>
+      </c>
+      <c r="O60" t="s">
+        <v>414</v>
+      </c>
+      <c r="P60" s="2">
+        <v>43061</v>
+      </c>
+      <c r="Q60" t="s">
         <v>415</v>
-      </c>
-      <c r="L60" t="s">
-        <v>416</v>
-      </c>
-      <c r="M60" t="s">
-        <v>417</v>
-      </c>
-      <c r="N60" t="s">
-        <v>24</v>
-      </c>
-      <c r="O60" t="s">
-        <v>24</v>
-      </c>
-      <c r="P60" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="2">
-        <v>43152</v>
+      <c r="B61" t="s">
+        <v>418</v>
       </c>
       <c r="C61" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D61" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I61" t="s">
         <v>59</v>
       </c>
       <c r="K61" t="s">
+        <v>419</v>
+      </c>
+      <c r="L61" t="s">
+        <v>420</v>
+      </c>
+      <c r="M61" t="s">
+        <v>24</v>
+      </c>
+      <c r="N61" t="s">
+        <v>24</v>
+      </c>
+      <c r="O61" t="s">
+        <v>421</v>
+      </c>
+      <c r="P61" s="2">
+        <v>43152</v>
+      </c>
+      <c r="Q61" t="s">
         <v>422</v>
-      </c>
-      <c r="L61" t="s">
-        <v>423</v>
-      </c>
-      <c r="M61" t="s">
-        <v>424</v>
-      </c>
-      <c r="N61" t="s">
-        <v>24</v>
-      </c>
-      <c r="O61" t="s">
-        <v>24</v>
-      </c>
-      <c r="P61" t="s">
-        <v>425</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" t="s">
+        <v>426</v>
+      </c>
+      <c r="C62" t="s">
+        <v>423</v>
+      </c>
+      <c r="D62" t="s">
+        <v>424</v>
+      </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
+        <v>425</v>
+      </c>
+      <c r="G62" t="s">
+        <v>116</v>
+      </c>
+      <c r="K62" t="s">
+        <v>427</v>
+      </c>
+      <c r="M62" t="s">
+        <v>24</v>
+      </c>
+      <c r="N62" t="s">
+        <v>24</v>
+      </c>
+      <c r="O62" t="s">
+        <v>428</v>
+      </c>
+      <c r="P62" s="2">
         <v>42914</v>
       </c>
-      <c r="C62" t="s">
-        <v>427</v>
-      </c>
-      <c r="D62" t="s">
-        <v>428</v>
-      </c>
-      <c r="E62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="Q62" t="s">
         <v>429</v>
-      </c>
-      <c r="K62" t="s">
-        <v>430</v>
-      </c>
-      <c r="L62" t="s">
-        <v>431</v>
-      </c>
-      <c r="N62" t="s">
-        <v>24</v>
-      </c>
-      <c r="O62" t="s">
-        <v>24</v>
-      </c>
-      <c r="P62" t="s">
-        <v>432</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" t="s">
+        <v>431</v>
+      </c>
+      <c r="C63" t="s">
+        <v>430</v>
+      </c>
+      <c r="D63" t="s">
+        <v>424</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>425</v>
+      </c>
+      <c r="G63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K63" t="s">
+        <v>242</v>
+      </c>
+      <c r="M63" t="s">
+        <v>24</v>
+      </c>
+      <c r="N63" t="s">
+        <v>24</v>
+      </c>
+      <c r="O63" t="s">
+        <v>432</v>
+      </c>
+      <c r="P63" s="2">
         <v>42914</v>
       </c>
-      <c r="C63" t="s">
-        <v>434</v>
-      </c>
-      <c r="D63" t="s">
-        <v>428</v>
-      </c>
-      <c r="E63" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" t="s">
-        <v>429</v>
-      </c>
-      <c r="K63" t="s">
-        <v>435</v>
-      </c>
-      <c r="L63" t="s">
-        <v>243</v>
-      </c>
-      <c r="N63" t="s">
-        <v>24</v>
-      </c>
-      <c r="O63" t="s">
-        <v>24</v>
-      </c>
-      <c r="P63" t="s">
-        <v>436</v>
-      </c>
       <c r="Q63" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="2">
-        <v>44539</v>
+      <c r="B64" t="s">
+        <v>436</v>
       </c>
       <c r="C64" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D64" t="s">
         <v>18</v>
@@ -4514,107 +4531,148 @@
         <v>74</v>
       </c>
       <c r="J64" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="K64" t="s">
-        <v>440</v>
-      </c>
-      <c r="L64" t="s">
-        <v>441</v>
+        <v>437</v>
+      </c>
+      <c r="M64" t="s">
+        <v>33</v>
       </c>
       <c r="N64" t="s">
         <v>33</v>
       </c>
       <c r="O64" t="s">
-        <v>33</v>
-      </c>
-      <c r="P64" t="s">
-        <v>442</v>
+        <v>438</v>
+      </c>
+      <c r="P64" s="2">
+        <v>44539</v>
       </c>
       <c r="Q64" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" t="s">
+        <v>443</v>
+      </c>
+      <c r="C65" t="s">
+        <v>440</v>
+      </c>
+      <c r="D65" t="s">
+        <v>441</v>
+      </c>
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" t="s">
+        <v>442</v>
+      </c>
+      <c r="K65" t="s">
+        <v>444</v>
+      </c>
+      <c r="L65" t="s">
+        <v>374</v>
+      </c>
+      <c r="M65" t="s">
+        <v>24</v>
+      </c>
+      <c r="N65" t="s">
+        <v>24</v>
+      </c>
+      <c r="O65" t="s">
+        <v>445</v>
+      </c>
+      <c r="P65" s="2">
         <v>45398</v>
       </c>
-      <c r="C65" t="s">
-        <v>444</v>
-      </c>
-      <c r="D65" t="s">
-        <v>445</v>
-      </c>
-      <c r="E65" t="s">
-        <v>19</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="Q65" t="s">
         <v>446</v>
-      </c>
-      <c r="K65" t="s">
-        <v>447</v>
-      </c>
-      <c r="L65" t="s">
-        <v>448</v>
-      </c>
-      <c r="M65" t="s">
-        <v>378</v>
-      </c>
-      <c r="N65" t="s">
-        <v>24</v>
-      </c>
-      <c r="O65" t="s">
-        <v>24</v>
-      </c>
-      <c r="P65" t="s">
-        <v>449</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="2">
-        <v>45412</v>
+      <c r="B66" t="s">
+        <v>449</v>
       </c>
       <c r="C66" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D66" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G66" t="s">
         <v>99</v>
       </c>
       <c r="K66" t="s">
+        <v>450</v>
+      </c>
+      <c r="M66" t="s">
+        <v>24</v>
+      </c>
+      <c r="N66" t="s">
+        <v>24</v>
+      </c>
+      <c r="O66" t="s">
+        <v>451</v>
+      </c>
+      <c r="P66" s="2">
+        <v>45412</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>453</v>
       </c>
-      <c r="L66" t="s">
+      <c r="C67" t="s">
         <v>454</v>
       </c>
-      <c r="N66" t="s">
-        <v>24</v>
-      </c>
-      <c r="O66" t="s">
-        <v>24</v>
-      </c>
-      <c r="P66" t="s">
+      <c r="D67" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" t="s">
+        <v>194</v>
+      </c>
+      <c r="H67" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67" t="s">
         <v>455</v>
       </c>
-      <c r="Q66" t="s">
-        <v>456</v>
+      <c r="K67" s="3">
+        <v>1.2847222222222222E-2</v>
+      </c>
+      <c r="L67" s="3">
+        <v>5.2685185185185182E-2</v>
+      </c>
+      <c r="M67" t="s">
+        <v>24</v>
+      </c>
+      <c r="N67" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>